<commit_message>
Finalisation of paper 07 for WPDCS20
</commit_message>
<xml_diff>
--- a/Data/Requests_to_WPDCS.xlsx
+++ b/Data/Requests_to_WPDCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-section-activities\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\working-parties\iotc-data-section-activities\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84565ED7-93E7-4CE2-AAD3-8931C731973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56809925-0CB7-4A68-A259-481690D451BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AEFAF3C7-4E28-4201-BEA8-128D069B6207}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AEFAF3C7-4E28-4201-BEA8-128D069B6207}"/>
   </bookViews>
   <sheets>
     <sheet name="detail" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>WPEB20(AS)</t>
   </si>
   <si>
-    <t>WPTT26 [Report not adopted yet]</t>
-  </si>
-  <si>
     <t>The WGEMS NOTED the intention of the Secretariat to repeat this exercise routinely in an automated way to better monitor the contents of the ROS database. The WGEMS REQUESTED the Secretariat to continue with this work</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>The WGEMS NOTED that geo-referenced catch, effort, and size-frequency data have been collected in Pakistan for the year 2022 but not yet transmitted to the Secretariat due to administrative issues. The WGEMS URGED Pakistan to report the data at their earliest convenience</t>
+  </si>
+  <si>
+    <t>WPTT26</t>
   </si>
 </sst>
 </file>
@@ -294,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,17 +321,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -886,19 +885,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDCD9A6-0F4A-4783-83C2-4AF73FFEFB8F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="179.42578125" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="25.1796875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="179.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -909,184 +907,184 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="10">
         <v>30</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="10">
         <v>146</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="10">
         <v>81</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="10">
         <v>34</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="10">
         <v>35</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="10">
         <v>36</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="10">
         <v>31</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="10">
         <v>11</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="10">
         <v>42</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="10">
         <v>12</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="10">
         <v>20</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="10">
         <v>51</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="10">
         <v>54</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="10">
         <v>152</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="10">
         <v>162</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B17" s="10">
         <v>78</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
+      <c r="C17" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C18" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C17" xr:uid="{CEDCD9A6-0F4A-4783-83C2-4AF73FFEFB8F}"/>
@@ -1102,14 +1100,14 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1123,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1133,7 +1131,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1141,7 +1139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1149,7 +1147,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1163,7 +1161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1191,7 +1189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1205,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -1233,7 +1231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1247,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -1261,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1297,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>7</v>
       </c>
@@ -1305,7 +1303,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
@@ -1313,7 +1311,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1321,7 +1319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>7</v>
       </c>
@@ -1329,7 +1327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
@@ -1337,7 +1335,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
         <v>9</v>
       </c>
@@ -1345,7 +1343,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -1353,7 +1351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -1361,7 +1359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
@@ -1369,7 +1367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
@@ -1377,7 +1375,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
@@ -1385,7 +1383,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
@@ -1393,7 +1391,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>